<commit_message>
introducing the attenuation factor
</commit_message>
<xml_diff>
--- a/Tables/NN_parameters_GPT_in.xlsx
+++ b/Tables/NN_parameters_GPT_in.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\NN_molecular_communications\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\NN_molecular_communications\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99FF065-0F3F-4422-B0AD-B92F4769E566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7671C85-36F9-4C6F-AF9A-827FEFB46706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A8CD4E30-4109-45FF-9D64-96F9252F4BB1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{A8CD4E30-4109-45FF-9D64-96F9252F4BB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="155">
   <si>
     <t>MC Geometry</t>
   </si>
@@ -153,15 +153,6 @@
     <t>\cite{qian2018receiver}</t>
   </si>
   <si>
-    <t>450 \milli \second</t>
-  </si>
-  <si>
-    <t>*-5 to 35</t>
-  </si>
-  <si>
-    <t>5e-1 to 2e-5</t>
-  </si>
-  <si>
     <t>5 \micro \meter</t>
   </si>
   <si>
@@ -471,10 +462,6 @@
     <t>\cite{bai2023temporal}</t>
   </si>
   <si>
-    <t>CNN and
-RNN</t>
-  </si>
-  <si>
     <t>1 \minute</t>
   </si>
   <si>
@@ -499,7 +486,25 @@
     <t>&lt; 85 \percent</t>
   </si>
   <si>
-    <t>\textcolor{red}{\cite{torres-gomez2021dna}}</t>
+    <t>\cite{ozdemir2021estimating}</t>
+  </si>
+  <si>
+    <t>\cite{torres-gomez2021dna-based</t>
+  </si>
+  <si>
+    <t>\cite{qian2018molecular}</t>
+  </si>
+  <si>
+    <t>\cite{farsad2018detection}</t>
+  </si>
+  <si>
+    <t>\cite{farsad2021datadriven}</t>
+  </si>
+  <si>
+    <t>\cite{cheng2023signal}</t>
+  </si>
+  <si>
+    <t>\cite{khanzadeh2023towards}</t>
   </si>
 </sst>
 </file>
@@ -935,7 +940,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -946,51 +951,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1000,9 +975,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1021,75 +993,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1102,36 +1020,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1144,12 +1038,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1162,104 +1050,314 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1595,17 +1693,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C57A639-0991-47E9-811D-E6882B262D04}">
-  <dimension ref="A1:Z1021"/>
+  <dimension ref="A1:Z1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:L1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.90625" style="87" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" style="87" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" style="99" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.90625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" style="45" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1796875" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" customWidth="1"/>
     <col min="6" max="6" width="13.54296875" customWidth="1"/>
@@ -1614,19 +1712,19 @@
     <col min="9" max="9" width="9.26953125" customWidth="1"/>
     <col min="10" max="10" width="8.26953125" customWidth="1"/>
     <col min="11" max="11" width="16.6328125" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="12" max="12" width="15" style="98" customWidth="1"/>
     <col min="13" max="13" width="10.26953125" customWidth="1"/>
     <col min="14" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1647,1190 +1745,1344 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="108"/>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="106" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="8">
-        <v>200</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="94" t="s">
+        <v>154</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="106" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="13">
-        <v>3000</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
+      <c r="A3" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="107">
+        <v>124000</v>
+      </c>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="126" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" s="94" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="106" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="13">
-        <v>3000</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
+      <c r="B4" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="108">
+        <v>0.79</v>
+      </c>
+      <c r="G4" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="106" t="s">
+      <c r="B5" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="107" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="107" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="18">
-        <v>0.42</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="20" t="s">
+      <c r="D5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="68">
+        <v>1</v>
+      </c>
+      <c r="G5" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
+      <c r="K5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="95" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="106" t="s">
+      <c r="B6" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="107" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="107" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="18">
-        <v>0.42</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="106" t="s">
+      <c r="B7" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="26">
-        <v>1.01</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>46</v>
-      </c>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="106" t="s">
+      <c r="A8" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="26">
-        <v>1.01</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="20" t="s">
+      <c r="D8" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="54"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="28" t="s">
-        <v>47</v>
-      </c>
+      <c r="K8" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="106" t="s">
+      <c r="A9" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="26">
-        <v>1.01</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="20" t="s">
+      <c r="D9" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="54"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" s="28" t="s">
-        <v>48</v>
-      </c>
+      <c r="K9" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="L9" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="101" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0.79</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="35" t="s">
-        <v>54</v>
+      <c r="A10" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="93">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="39">
-        <v>25</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="L11" s="42" t="s">
-        <v>61</v>
+      <c r="A11" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="15">
+        <v>0.84</v>
+      </c>
+      <c r="G11" s="117">
+        <v>4.9000000000000003E+23</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="I11" s="16">
+        <v>27.5</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="43">
-        <v>0.06</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" s="45" t="s">
-        <v>68</v>
+      <c r="A12" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12" s="43"/>
+      <c r="J12" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="K12" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="L12" s="97" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="104" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="48">
-        <v>25</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="K13" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="L13" s="42" t="s">
-        <v>61</v>
+      <c r="A13" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="L13" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="101" t="s">
+      <c r="A14" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="104" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="106" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="30">
-        <v>0.79</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="L14" s="28" t="s">
-        <v>75</v>
+      <c r="B14" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="33" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="106" t="s">
+      <c r="A15" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="43">
-        <v>1</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="53" t="s">
+      <c r="D15" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="G15" s="116" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="116" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="K15" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="45" t="s">
-        <v>82</v>
+      <c r="K15" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="106" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="43">
-        <v>5</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="I16" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="L16" s="45" t="s">
-        <v>89</v>
+      <c r="A16" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="56"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="I16" s="56"/>
+      <c r="J16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="132">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="106" t="s">
+      <c r="A17" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="43">
-        <v>5</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="53" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="54"/>
+      <c r="J17" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="K17" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="L17" s="45" t="s">
-        <v>90</v>
+      <c r="K17" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="106" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="55">
-        <v>0.79</v>
-      </c>
-      <c r="G18" s="56">
-        <v>4000</v>
-      </c>
-      <c r="H18" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="I18" s="57" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="L18" s="58" t="s">
-        <v>96</v>
+      <c r="A18" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="60"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="L18" s="138" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="74" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="106" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="59">
-        <v>124000</v>
-      </c>
-      <c r="G19" s="57"/>
-      <c r="H19" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="I19" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="J19" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="L19" s="58" t="s">
-        <v>101</v>
+      <c r="A19" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="K19" s="133" t="s">
+        <v>147</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="101" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="103" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61">
-        <v>0.1</v>
-      </c>
-      <c r="G20" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="I20" s="62"/>
-      <c r="J20" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="K20" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="L20" s="64" t="s">
-        <v>108</v>
+      <c r="A20" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="19">
+        <v>1.01</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="101" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="57"/>
-      <c r="J21" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="L21" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="M21" s="67"/>
-      <c r="N21" s="67"/>
-      <c r="O21" s="67"/>
-      <c r="P21" s="67"/>
-      <c r="Q21" s="67"/>
-      <c r="R21" s="67"/>
-      <c r="S21" s="67"/>
-      <c r="T21" s="67"/>
-      <c r="U21" s="67"/>
-      <c r="V21" s="67"/>
-      <c r="W21" s="67"/>
-      <c r="X21" s="67"/>
-      <c r="Y21" s="67"/>
-      <c r="Z21" s="67"/>
+      <c r="A21" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="114">
+        <v>0.79</v>
+      </c>
+      <c r="G21" s="103" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="60"/>
+      <c r="J21" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="131" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="139" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="101" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="I22" s="68"/>
-      <c r="J22" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="71">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="L22" s="72" t="s">
-        <v>113</v>
-      </c>
-      <c r="M22" s="67"/>
-      <c r="N22" s="67"/>
-      <c r="O22" s="67"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="67"/>
-      <c r="T22" s="67"/>
-      <c r="U22" s="67"/>
-      <c r="V22" s="67"/>
-      <c r="W22" s="67"/>
-      <c r="X22" s="67"/>
-      <c r="Y22" s="67"/>
-      <c r="Z22" s="67"/>
+      <c r="A22" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="112" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="119">
+        <v>3000</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="137" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="101" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="103" t="s">
+      <c r="A23" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="25"/>
-      <c r="J23" s="67" t="s">
+      <c r="D23" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="71">
+        <v>0.42</v>
+      </c>
+      <c r="G23" s="118"/>
+      <c r="H23" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="K23" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="L23" s="73" t="s">
-        <v>116</v>
+      <c r="K23" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="33" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
+    </row>
+    <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="32">
+        <v>0.06</v>
+      </c>
+      <c r="G25" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="84" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="L25" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="30"/>
+      <c r="Z25" s="30"/>
+    </row>
+    <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="81">
+        <v>25</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="L28" s="96" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A29" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="41" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="74">
+        <v>3000</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="127" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="41" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="110" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="91">
+        <v>200</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="92" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="135" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" s="41" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="102" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="102" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="111" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="65"/>
+      <c r="H32" s="121" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="123">
+        <v>25</v>
+      </c>
+      <c r="J32" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="130" t="s">
+        <v>67</v>
+      </c>
+      <c r="L32" s="136" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="100" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="105"/>
+      <c r="F33" s="109">
+        <v>0.1</v>
+      </c>
+      <c r="G33" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="103" t="s">
+      <c r="I33" s="122"/>
+      <c r="J33" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="K33" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="L33" s="97" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D34" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="L34" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="I24" s="25"/>
-      <c r="J24" s="67" t="s">
+    </row>
+    <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="36">
+        <v>5</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J35" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="L24" s="73" t="s">
-        <v>117</v>
+      <c r="K35" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A25" s="101" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" s="74" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="103" t="s">
+    <row r="36" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="I25" s="32"/>
-      <c r="J25" s="77" t="s">
-        <v>121</v>
-      </c>
-      <c r="K25" s="76" t="s">
-        <v>122</v>
-      </c>
-      <c r="L25" s="78" t="s">
-        <v>123</v>
+      <c r="D36" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="37">
+        <v>5</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J36" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A26" s="101" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="74" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" s="103" t="s">
+    <row r="37" spans="1:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="80" t="s">
+      <c r="D37" s="104" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="104" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="115">
+        <v>0.79</v>
+      </c>
+      <c r="G37" s="120">
+        <v>4000</v>
+      </c>
+      <c r="H37" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="125" t="s">
+        <v>91</v>
+      </c>
+      <c r="J37" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="K26" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="L26" s="28" t="s">
-        <v>127</v>
+      <c r="K37" s="134" t="s">
+        <v>92</v>
+      </c>
+      <c r="L37" s="44" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:26" s="87" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="102" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" s="74" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="81" t="s">
-        <v>129</v>
-      </c>
-      <c r="E27" s="81"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="83" t="s">
-        <v>130</v>
-      </c>
-      <c r="I27" s="81"/>
-      <c r="J27" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="85">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L27" s="86" t="s">
-        <v>131</v>
+    <row r="38" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="17" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="102" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="43">
-        <v>0.84</v>
-      </c>
-      <c r="G28" s="88">
-        <v>4.9000000000000003E+23</v>
-      </c>
-      <c r="H28" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="I28" s="57">
-        <v>27.5</v>
-      </c>
-      <c r="J28" s="89" t="s">
-        <v>34</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="L28" s="28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="101" t="s">
-        <v>136</v>
-      </c>
-      <c r="B29" s="74" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29" s="55">
-        <v>0.75</v>
-      </c>
-      <c r="G29" s="90" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" s="91" t="s">
-        <v>140</v>
-      </c>
-      <c r="I29" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="J29" s="89" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="L29" s="73" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="101" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="74" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="I30" s="27"/>
-      <c r="J30" s="89" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="L30" s="28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="105" t="s">
-        <v>147</v>
-      </c>
-      <c r="B31" s="105" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="92"/>
-      <c r="J31" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="K31" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="L31" s="94" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="105" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="105" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="105" t="s">
-        <v>150</v>
-      </c>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="95" t="s">
-        <v>73</v>
-      </c>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95" t="s">
-        <v>121</v>
-      </c>
-      <c r="K32" s="97" t="s">
-        <v>151</v>
-      </c>
-      <c r="L32" s="98" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3804,9 +4056,17 @@
     <row r="1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1020" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1021" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1022" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1023" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1024" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1025" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1026" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <autoFilter ref="A1:L32" xr:uid="{5C57A639-0991-47E9-811D-E6882B262D04}">
+  <autoFilter ref="A1:L37" xr:uid="{5C57A639-0991-47E9-811D-E6882B262D04}">
     <filterColumn colId="9" showButton="0"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L37">
+      <sortCondition ref="B1:B37"/>
+    </sortState>
   </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>

</xml_diff>